<commit_message>
Update Excel file via API
</commit_message>
<xml_diff>
--- a/python/BytheNumbersWorksheet.xlsx
+++ b/python/BytheNumbersWorksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baskausj/Documents/GitHub/dashboard/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63F3003-00D8-B045-A8A2-C0936E2C65CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E0A0E9-7EAE-AF45-8776-AB11FF505D34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14780" yWindow="1300" windowWidth="28800" windowHeight="12040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14780" yWindow="1300" windowWidth="28800" windowHeight="12040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rankings" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>Instructional Sessions</t>
   </si>
   <si>
-    <t xml:space="preserve">Ed Tech/Digital Literacy Instructional Sessions </t>
-  </si>
-  <si>
     <t>Attendees at all events</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>inverseRank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ed Tech / Digital Literacy Instructional Sessions </t>
   </si>
 </sst>
 </file>
@@ -641,7 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -652,7 +652,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2003</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N3">
         <v>114</v>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -803,7 +803,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -856,7 +856,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3">
         <v>15388</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2">
         <v>8869</v>
@@ -903,7 +903,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="3">
         <v>2376301</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3">
         <v>2969957</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>8524</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3">
         <v>1118709</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3">
         <v>39627</v>
@@ -985,7 +985,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
@@ -1047,7 +1047,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -1059,7 +1059,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -1071,7 +1071,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
@@ -1083,7 +1083,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -1113,7 +1113,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1">
         <v>2020</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>19.850000000000001</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>76.67</v>
@@ -1143,7 +1143,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>3.48</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="10">
         <v>11</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="10">
         <v>86</v>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="10">
         <v>3</v>
@@ -1195,7 +1195,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -1206,22 +1206,22 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="5">
         <v>109636</v>
@@ -1229,7 +1229,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="5">
         <v>43287</v>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="5">
         <v>7524</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="5">
         <v>17313</v>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="5">
         <v>26481</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5">
         <v>20589</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="5">
         <v>10633</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="5">
         <v>38535</v>
@@ -1285,7 +1285,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="5">
         <v>37557</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="14" spans="1:3" ht="16" thickBot="1">
       <c r="A14" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="7">
         <f t="shared" ref="B14" si="0">SUM(B5:B13)</f>
@@ -1320,7 +1320,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3">
         <v>1045017</v>
@@ -1366,7 +1366,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -1377,37 +1377,37 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1431,7 +1431,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2">
         <v>979</v>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>320</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4">
         <v>866</v>
@@ -1474,6 +1474,39 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2">
+      <UserInfo>
+        <DisplayName>Baskauf, Steven James</DisplayName>
+        <AccountId>331</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>You, Tao</DisplayName>
+        <AccountId>39</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Carnes, Taylor</DisplayName>
+        <AccountId>556</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BFBD00BD3A3E1E4A988918AADBA3442C" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="88f30bb8313cbfe73ab7c84b296b4218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ffda594d-e23b-4583-b5d5-0ebe66b53dbd" xmlns:ns3="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04f1bc45e0fc885fdfc66bf71deb596f" ns2:_="" ns3:_="">
     <xsd:import namespace="ffda594d-e23b-4583-b5d5-0ebe66b53dbd"/>
@@ -1638,40 +1671,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2">
-      <UserInfo>
-        <DisplayName>Baskauf, Steven James</DisplayName>
-        <AccountId>331</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>You, Tao</DisplayName>
-        <AccountId>39</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Carnes, Taylor</DisplayName>
-        <AccountId>556</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F54041C0-C8B4-442E-B92E-3FCFCD1EF89D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00D6D499-0000-4C85-8F24-AD9A81FFD6C2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7953FC9-F19D-4967-A378-149CD58E2AD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1688,22 +1706,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00D6D499-0000-4C85-8F24-AD9A81FFD6C2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F54041C0-C8B4-442E-B92E-3FCFCD1EF89D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update script to backup Excel file (Issue #4)
</commit_message>
<xml_diff>
--- a/python/BytheNumbersWorksheet.xlsx
+++ b/python/BytheNumbersWorksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baskausj/Documents/GitHub/dashboard/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63F3003-00D8-B045-A8A2-C0936E2C65CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E0A0E9-7EAE-AF45-8776-AB11FF505D34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14780" yWindow="1300" windowWidth="28800" windowHeight="12040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14780" yWindow="1300" windowWidth="28800" windowHeight="12040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rankings" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>Instructional Sessions</t>
   </si>
   <si>
-    <t xml:space="preserve">Ed Tech/Digital Literacy Instructional Sessions </t>
-  </si>
-  <si>
     <t>Attendees at all events</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>inverseRank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ed Tech / Digital Literacy Instructional Sessions </t>
   </si>
 </sst>
 </file>
@@ -641,7 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -652,7 +652,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2003</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N3">
         <v>114</v>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -803,7 +803,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -856,7 +856,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3">
         <v>15388</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2">
         <v>8869</v>
@@ -903,7 +903,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="3">
         <v>2376301</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3">
         <v>2969957</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>8524</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3">
         <v>1118709</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3">
         <v>39627</v>
@@ -985,7 +985,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
@@ -1047,7 +1047,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -1059,7 +1059,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -1071,7 +1071,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
@@ -1083,7 +1083,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -1113,7 +1113,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1">
         <v>2020</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>19.850000000000001</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>76.67</v>
@@ -1143,7 +1143,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>3.48</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="10">
         <v>11</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="10">
         <v>86</v>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="10">
         <v>3</v>
@@ -1195,7 +1195,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -1206,22 +1206,22 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="5">
         <v>109636</v>
@@ -1229,7 +1229,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="5">
         <v>43287</v>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="5">
         <v>7524</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="5">
         <v>17313</v>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="5">
         <v>26481</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5">
         <v>20589</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="5">
         <v>10633</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="5">
         <v>38535</v>
@@ -1285,7 +1285,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="5">
         <v>37557</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="14" spans="1:3" ht="16" thickBot="1">
       <c r="A14" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="7">
         <f t="shared" ref="B14" si="0">SUM(B5:B13)</f>
@@ -1320,7 +1320,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3">
         <v>1045017</v>
@@ -1366,7 +1366,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -1377,37 +1377,37 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1431,7 +1431,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2">
         <v>979</v>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>320</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4">
         <v>866</v>
@@ -1474,6 +1474,39 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2">
+      <UserInfo>
+        <DisplayName>Baskauf, Steven James</DisplayName>
+        <AccountId>331</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>You, Tao</DisplayName>
+        <AccountId>39</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Carnes, Taylor</DisplayName>
+        <AccountId>556</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BFBD00BD3A3E1E4A988918AADBA3442C" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="88f30bb8313cbfe73ab7c84b296b4218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ffda594d-e23b-4583-b5d5-0ebe66b53dbd" xmlns:ns3="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04f1bc45e0fc885fdfc66bf71deb596f" ns2:_="" ns3:_="">
     <xsd:import namespace="ffda594d-e23b-4583-b5d5-0ebe66b53dbd"/>
@@ -1638,40 +1671,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2">
-      <UserInfo>
-        <DisplayName>Baskauf, Steven James</DisplayName>
-        <AccountId>331</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>You, Tao</DisplayName>
-        <AccountId>39</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Carnes, Taylor</DisplayName>
-        <AccountId>556</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F54041C0-C8B4-442E-B92E-3FCFCD1EF89D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00D6D499-0000-4C85-8F24-AD9A81FFD6C2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7953FC9-F19D-4967-A378-149CD58E2AD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1688,22 +1706,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00D6D499-0000-4C85-8F24-AD9A81FFD6C2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F54041C0-C8B4-442E-B92E-3FCFCD1EF89D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GUI code completed (Issue #2)
</commit_message>
<xml_diff>
--- a/python/BytheNumbersWorksheet.xlsx
+++ b/python/BytheNumbersWorksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baskausj/Documents/GitHub/dashboard/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E0A0E9-7EAE-AF45-8776-AB11FF505D34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C0A4F6-E152-734A-AD04-E69B31A9A9FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14780" yWindow="1300" windowWidth="28800" windowHeight="12040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14780" yWindow="1300" windowWidth="28800" windowHeight="12040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rankings" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -59,12 +59,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-file:///G:\LIBADMIN_STATISTICS\Collections\Archives%20Linear%20Measurements.xlsx</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>file:///G:\LIBADMIN_STATISTICS\Collections\Archives%20Linear%20Measurements.xlsx</t>
         </r>
       </text>
     </comment>
@@ -102,9 +111,6 @@
     <t>TVNA video segments</t>
   </si>
   <si>
-    <t>Special Collections &amp; University Archives, linear footage</t>
-  </si>
-  <si>
     <t>Total Circulation</t>
   </si>
   <si>
@@ -226,6 +232,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ed Tech / Digital Literacy Instructional Sessions </t>
+  </si>
+  <si>
+    <t>Special Collections and University Archives, linear footage</t>
   </si>
 </sst>
 </file>
@@ -269,15 +278,15 @@
       <name val="Source Sans Pro"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -652,7 +661,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1">
         <v>2003</v>
@@ -764,7 +773,7 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N3">
         <v>114</v>
@@ -788,7 +797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -803,7 +812,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -847,7 +856,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -892,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -903,7 +912,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -955,7 +964,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C6" s="3">
         <v>39627</v>
@@ -985,7 +994,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -999,7 +1008,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1009,7 +1018,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1019,7 +1028,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1029,7 +1038,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1037,7 +1046,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
@@ -1047,7 +1056,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -1059,7 +1068,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -1071,7 +1080,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
@@ -1083,7 +1092,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -1113,7 +1122,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1">
         <v>2020</v>
@@ -1127,7 +1136,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>19.850000000000001</v>
@@ -1135,7 +1144,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3">
         <v>76.67</v>
@@ -1143,7 +1152,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>3.48</v>
@@ -1151,7 +1160,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="10">
         <v>11</v>
@@ -1159,7 +1168,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="10">
         <v>86</v>
@@ -1167,7 +1176,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="10">
         <v>3</v>
@@ -1195,7 +1204,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -1206,22 +1215,22 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="5">
         <v>109636</v>
@@ -1229,7 +1238,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="5">
         <v>43287</v>
@@ -1237,7 +1246,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="5">
         <v>7524</v>
@@ -1245,7 +1254,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="5">
         <v>17313</v>
@@ -1253,7 +1262,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="5">
         <v>26481</v>
@@ -1261,7 +1270,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="5">
         <v>20589</v>
@@ -1269,7 +1278,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="5">
         <v>10633</v>
@@ -1277,7 +1286,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="5">
         <v>38535</v>
@@ -1285,7 +1294,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="5">
         <v>37557</v>
@@ -1293,7 +1302,7 @@
     </row>
     <row r="14" spans="1:3" ht="16" thickBot="1">
       <c r="A14" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="7">
         <f t="shared" ref="B14" si="0">SUM(B5:B13)</f>
@@ -1320,7 +1329,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -1337,7 +1346,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3">
         <v>1045017</v>
@@ -1366,7 +1375,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -1377,32 +1386,32 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1431,7 +1440,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -1445,7 +1454,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>979</v>
@@ -1453,7 +1462,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3">
         <v>320</v>
@@ -1461,7 +1470,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4">
         <v>866</v>
@@ -1474,6 +1483,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2">
@@ -1495,15 +1513,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1672,19 +1681,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00D6D499-0000-4C85-8F24-AD9A81FFD6C2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F54041C0-C8B4-442E-B92E-3FCFCD1EF89D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00D6D499-0000-4C85-8F24-AD9A81FFD6C2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
remove initial blank row from Collections sheet in Excel file
</commit_message>
<xml_diff>
--- a/python/BytheNumbersWorksheet.xlsx
+++ b/python/BytheNumbersWorksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lannomla\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baskausj/Documents/GitHub/dashboard/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F68BF6-E683-40C2-9B44-6D30814890BE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79775A1B-2415-3745-9A15-A81B4D7C8415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rankings" sheetId="1" r:id="rId1"/>
@@ -506,12 +506,12 @@
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -519,7 +519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2003</v>
       </c>
@@ -527,7 +527,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2004</v>
       </c>
@@ -535,7 +535,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2005</v>
       </c>
@@ -543,7 +543,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2006</v>
       </c>
@@ -551,7 +551,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2007</v>
       </c>
@@ -559,7 +559,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2008</v>
       </c>
@@ -567,7 +567,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2009</v>
       </c>
@@ -575,7 +575,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2010</v>
       </c>
@@ -583,7 +583,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -591,7 +591,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2012</v>
       </c>
@@ -599,7 +599,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2013</v>
       </c>
@@ -607,7 +607,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2014</v>
       </c>
@@ -615,7 +615,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2015</v>
       </c>
@@ -623,7 +623,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2016</v>
       </c>
@@ -631,7 +631,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2017</v>
       </c>
@@ -639,7 +639,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2018</v>
       </c>
@@ -660,15 +660,15 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -682,7 +682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -696,7 +696,7 @@
         <v>8869</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -710,7 +710,7 @@
         <v>7603</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2017</v>
       </c>
@@ -732,79 +732,79 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2019</v>
+      </c>
+      <c r="B2" s="8">
+        <v>9999999</v>
+      </c>
+      <c r="C2" s="8">
+        <v>9999999</v>
+      </c>
+      <c r="D2" s="8">
+        <v>8524</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1118709</v>
+      </c>
+      <c r="F2" s="8">
+        <v>39627</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2019</v>
-      </c>
-      <c r="B3" s="8">
-        <v>9999999</v>
-      </c>
-      <c r="C3" s="8">
-        <v>9999999</v>
-      </c>
-      <c r="D3" s="8">
-        <v>8524</v>
-      </c>
-      <c r="E3" s="8">
-        <v>1118709</v>
-      </c>
-      <c r="F3" s="8">
-        <v>39627</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
         <v>2018</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B3" s="3">
         <v>2376301</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C3" s="3">
         <v>2969957</v>
       </c>
-      <c r="D4">
+      <c r="D3">
         <v>8323</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E3" s="3">
         <v>1107223</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F3" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -819,21 +819,21 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -865,7 +865,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -897,7 +897,7 @@
         <v>7383</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -937,18 +937,18 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -971,12 +971,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2018</v>
       </c>
@@ -1013,17 +1013,17 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -1070,13 +1070,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>1206444</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>1045017</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2017</v>
       </c>
@@ -1121,13 +1121,13 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -1153,19 +1153,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1214,6 +1214,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2">
@@ -1235,15 +1244,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1412,6 +1412,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00D6D499-0000-4C85-8F24-AD9A81FFD6C2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F54041C0-C8B4-442E-B92E-3FCFCD1EF89D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1424,14 +1432,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="a63f8c51-8f9e-4dd1-b6cd-8c5ff29615d2"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00D6D499-0000-4C85-8F24-AD9A81FFD6C2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>